<commit_message>
Main update: proteome models generated
</commit_message>
<xml_diff>
--- a/ecCollab/data/Sample_Data.xlsx
+++ b/ecCollab/data/Sample_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecCollab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFCBB4C-7A4F-4B93-9031-CE7D8F355981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914231D9-AA31-43BA-AE31-0524560635DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{3171616A-1048-884C-94E3-682E97848501}"/>
+    <workbookView xWindow="3650" yWindow="14290" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{3171616A-1048-884C-94E3-682E97848501}"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="3" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -283,9 +283,6 @@
     <t>qItaconate mmol gCDW-1 h-1</t>
   </si>
   <si>
-    <t>JFYL66</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
@@ -626,6 +623,9 @@
   </si>
   <si>
     <t>rxns</t>
+  </si>
+  <si>
+    <t>JFYL14</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -675,11 +675,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -709,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -718,9 +713,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -735,7 +727,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -744,7 +736,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,14 +854,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Juliano Sabedotti De Biaggi" refreshedDate="45272.971093287037" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{9C69830B-CC26-4273-B036-50A5B227DCBB}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Juliano Sabedotti De Biaggi" refreshedDate="45327.716639467595" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{9C69830B-CC26-4273-B036-50A5B227DCBB}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="13">
     <cacheField name="[Table1].[Strain].[Strain]" caption="Strain" numFmtId="0" level="1">
       <sharedItems count="5">
         <s v="JFYL07"/>
+        <s v="JFYL14"/>
         <s v="JFYL18"/>
-        <s v="JFYL66"/>
         <s v="OKYL029"/>
         <s v="ST6512"/>
       </sharedItems>
@@ -1174,18 +1166,19 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Juliano Sabedotti De Biaggi" refreshedDate="45273.672683101853" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="19" xr:uid="{5C82F358-6549-4DF6-B701-813678CD7A75}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Juliano Sabedotti De Biaggi" refreshedDate="45327.716679282406" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="19" xr:uid="{5C82F358-6549-4DF6-B701-813678CD7A75}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="54">
     <cacheField name="Strain" numFmtId="0">
-      <sharedItems count="5">
+      <sharedItems count="6">
         <s v="ST6512"/>
         <s v="OKYL029"/>
         <s v="JFYL07"/>
         <s v="JFYL18"/>
-        <s v="JFYL66"/>
+        <s v="JFYL14"/>
+        <s v="JFYL66" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Nitrogen source" numFmtId="0">
@@ -2426,143 +2419,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{99095EC4-0AC8-44E7-A94B-389D4A849554}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A8:G13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="54">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="2" showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField dataField="1" numFmtId="2" showAll="0"/>
-    <pivotField dataField="1" numFmtId="2" showAll="0"/>
-    <pivotField dataField="1" numFmtId="2" showAll="0"/>
-    <pivotField dataField="1" numFmtId="2" showAll="0"/>
-    <pivotField dataField="1" numFmtId="2" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
-  </colItems>
-  <dataFields count="6">
-    <dataField name="lipidCont" fld="24" subtotal="average" baseField="0" baseItem="0" numFmtId="166"/>
-    <dataField name="C16:0(m/m)" fld="30" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="C16:1(m/m)" fld="31" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="C18:0(m/m)" fld="32" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="C18:1(m/m)" fld="33" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="C18:2(m/m)" fld="34" subtotal="average" baseField="0" baseItem="1"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{56BAD6C6-E3B0-42CA-8E1B-5BE246750723}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{56BAD6C6-E3B0-42CA-8E1B-5BE246750723}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:M6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField name="Condition" axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -2663,7 +2520,7 @@
     <dataField name="itaconate ()" fld="12" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
@@ -2771,6 +2628,143 @@
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
       <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{99095EC4-0AC8-44E7-A94B-389D4A849554}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A8:G13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="54">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="2"/>
+        <item x="3"/>
+        <item m="1" x="5"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="lipidCont" fld="24" subtotal="average" baseField="0" baseItem="0" numFmtId="166"/>
+    <dataField name="C16:0(m/m)" fld="30" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="C16:1(m/m)" fld="31" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="C18:0(m/m)" fld="32" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="C18:1(m/m)" fld="33" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="C18:2(m/m)" fld="34" subtotal="average" baseField="0" baseItem="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -3183,8 +3177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93331D45-40EB-7947-9D79-F347D6495274}">
   <dimension ref="A1:BB48"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="AT8" sqref="AT8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3212,167 +3206,167 @@
     <col min="54" max="54" width="27.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="9" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:54" s="8" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AF1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AG1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AH1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AI1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AJ1" s="10" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AK1" s="10" t="s">
+      <c r="AK1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AL1" s="10" t="s">
+      <c r="AL1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AM1" s="10" t="s">
+      <c r="AM1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AN1" s="10" t="s">
+      <c r="AN1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AO1" s="10" t="s">
+      <c r="AO1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AP1" s="10" t="s">
+      <c r="AP1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" s="10" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AR1" s="10" t="s">
+      <c r="AR1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="12" t="s">
+      <c r="AS1" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AT1" s="10" t="s">
+      <c r="AT1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AU1" s="10" t="s">
+      <c r="AU1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AV1" s="10" t="s">
+      <c r="AV1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AW1" s="10" t="s">
+      <c r="AW1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AX1" s="10" t="s">
+      <c r="AX1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AY1" s="10" t="s">
+      <c r="AY1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AZ1" s="12" t="s">
+      <c r="AZ1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="BA1" s="10" t="s">
+      <c r="BA1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="BB1" s="9" t="s">
+      <c r="BB1" s="8" t="s">
         <v>51</v>
       </c>
     </row>
@@ -6270,8 +6264,8 @@
       </c>
     </row>
     <row r="18" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>59</v>
+      <c r="A18" t="s">
+        <v>173</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
@@ -6451,8 +6445,8 @@
       </c>
     </row>
     <row r="19" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>59</v>
+      <c r="A19" t="s">
+        <v>173</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
@@ -6629,8 +6623,8 @@
       </c>
     </row>
     <row r="20" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>59</v>
+      <c r="A20" t="s">
+        <v>173</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
@@ -6816,12 +6810,12 @@
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
       <c r="AE24" s="3"/>
-      <c r="AF24" s="11"/>
-      <c r="AG24" s="11"/>
-      <c r="AH24" s="11"/>
-      <c r="AI24" s="11"/>
-      <c r="AJ24" s="11"/>
-      <c r="AK24" s="11"/>
+      <c r="AF24" s="10"/>
+      <c r="AG24" s="10"/>
+      <c r="AH24" s="10"/>
+      <c r="AI24" s="10"/>
+      <c r="AJ24" s="10"/>
+      <c r="AK24" s="10"/>
     </row>
     <row r="25" spans="1:54" x14ac:dyDescent="0.25">
       <c r="Z25" s="3"/>
@@ -6830,12 +6824,12 @@
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
       <c r="AE25" s="3"/>
-      <c r="AF25" s="11"/>
-      <c r="AG25" s="11"/>
-      <c r="AH25" s="11"/>
-      <c r="AI25" s="11"/>
-      <c r="AJ25" s="11"/>
-      <c r="AK25" s="11"/>
+      <c r="AF25" s="10"/>
+      <c r="AG25" s="10"/>
+      <c r="AH25" s="10"/>
+      <c r="AI25" s="10"/>
+      <c r="AJ25" s="10"/>
+      <c r="AK25" s="10"/>
     </row>
     <row r="26" spans="1:54" x14ac:dyDescent="0.25">
       <c r="Z26" s="3"/>
@@ -6844,12 +6838,12 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
-      <c r="AF26" s="11"/>
-      <c r="AG26" s="11"/>
-      <c r="AH26" s="11"/>
-      <c r="AI26" s="11"/>
-      <c r="AJ26" s="11"/>
-      <c r="AK26" s="11"/>
+      <c r="AF26" s="10"/>
+      <c r="AG26" s="10"/>
+      <c r="AH26" s="10"/>
+      <c r="AI26" s="10"/>
+      <c r="AJ26" s="10"/>
+      <c r="AK26" s="10"/>
     </row>
     <row r="27" spans="1:54" x14ac:dyDescent="0.25">
       <c r="Z27" s="3"/>
@@ -6858,12 +6852,12 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
       <c r="AE27" s="3"/>
-      <c r="AF27" s="11"/>
-      <c r="AG27" s="11"/>
-      <c r="AH27" s="11"/>
-      <c r="AI27" s="11"/>
-      <c r="AJ27" s="11"/>
-      <c r="AK27" s="11"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="10"/>
+      <c r="AH27" s="10"/>
+      <c r="AI27" s="10"/>
+      <c r="AJ27" s="10"/>
+      <c r="AK27" s="10"/>
     </row>
     <row r="28" spans="1:54" x14ac:dyDescent="0.25">
       <c r="Z28" s="5"/>
@@ -6872,12 +6866,12 @@
       <c r="AC28" s="5"/>
       <c r="AD28" s="5"/>
       <c r="AE28" s="3"/>
-      <c r="AF28" s="11"/>
-      <c r="AG28" s="11"/>
-      <c r="AH28" s="11"/>
-      <c r="AI28" s="11"/>
-      <c r="AJ28" s="11"/>
-      <c r="AK28" s="11"/>
+      <c r="AF28" s="10"/>
+      <c r="AG28" s="10"/>
+      <c r="AH28" s="10"/>
+      <c r="AI28" s="10"/>
+      <c r="AJ28" s="10"/>
+      <c r="AK28" s="10"/>
     </row>
     <row r="29" spans="1:54" x14ac:dyDescent="0.25">
       <c r="Z29" s="3"/>
@@ -6886,12 +6880,12 @@
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
-      <c r="AF29" s="11"/>
-      <c r="AG29" s="11"/>
-      <c r="AH29" s="11"/>
-      <c r="AI29" s="11"/>
-      <c r="AJ29" s="11"/>
-      <c r="AK29" s="11"/>
+      <c r="AF29" s="10"/>
+      <c r="AG29" s="10"/>
+      <c r="AH29" s="10"/>
+      <c r="AI29" s="10"/>
+      <c r="AJ29" s="10"/>
+      <c r="AK29" s="10"/>
     </row>
     <row r="30" spans="1:54" x14ac:dyDescent="0.25">
       <c r="Y30" s="3"/>
@@ -6900,12 +6894,12 @@
       <c r="AB30" s="3"/>
       <c r="AD30" s="3"/>
       <c r="AE30" s="3"/>
-      <c r="AF30" s="11"/>
-      <c r="AG30" s="11"/>
-      <c r="AH30" s="11"/>
-      <c r="AI30" s="11"/>
-      <c r="AJ30" s="11"/>
-      <c r="AK30" s="11"/>
+      <c r="AF30" s="10"/>
+      <c r="AG30" s="10"/>
+      <c r="AH30" s="10"/>
+      <c r="AI30" s="10"/>
+      <c r="AJ30" s="10"/>
+      <c r="AK30" s="10"/>
     </row>
     <row r="31" spans="1:54" x14ac:dyDescent="0.25">
       <c r="Y31" s="3"/>
@@ -6914,12 +6908,12 @@
       <c r="AB31" s="3"/>
       <c r="AD31" s="3"/>
       <c r="AE31" s="3"/>
-      <c r="AF31" s="11"/>
-      <c r="AG31" s="11"/>
-      <c r="AH31" s="11"/>
-      <c r="AI31" s="11"/>
-      <c r="AJ31" s="11"/>
-      <c r="AK31" s="11"/>
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="10"/>
+      <c r="AH31" s="10"/>
+      <c r="AI31" s="10"/>
+      <c r="AJ31" s="10"/>
+      <c r="AK31" s="10"/>
     </row>
     <row r="32" spans="1:54" x14ac:dyDescent="0.25">
       <c r="Y32" s="3"/>
@@ -6928,12 +6922,12 @@
       <c r="AB32" s="3"/>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
-      <c r="AF32" s="11"/>
-      <c r="AG32" s="11"/>
-      <c r="AH32" s="11"/>
-      <c r="AI32" s="11"/>
-      <c r="AJ32" s="11"/>
-      <c r="AK32" s="11"/>
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="10"/>
+      <c r="AH32" s="10"/>
+      <c r="AI32" s="10"/>
+      <c r="AJ32" s="10"/>
+      <c r="AK32" s="10"/>
     </row>
     <row r="33" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y33" s="3"/>
@@ -6942,12 +6936,12 @@
       <c r="AB33" s="3"/>
       <c r="AD33" s="3"/>
       <c r="AE33" s="3"/>
-      <c r="AF33" s="11"/>
-      <c r="AG33" s="11"/>
-      <c r="AH33" s="11"/>
-      <c r="AI33" s="11"/>
-      <c r="AJ33" s="11"/>
-      <c r="AK33" s="11"/>
+      <c r="AF33" s="10"/>
+      <c r="AG33" s="10"/>
+      <c r="AH33" s="10"/>
+      <c r="AI33" s="10"/>
+      <c r="AJ33" s="10"/>
+      <c r="AK33" s="10"/>
     </row>
     <row r="34" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y34" s="5"/>
@@ -6956,12 +6950,12 @@
       <c r="AB34" s="3"/>
       <c r="AD34" s="3"/>
       <c r="AE34" s="3"/>
-      <c r="AF34" s="11"/>
-      <c r="AG34" s="11"/>
-      <c r="AH34" s="11"/>
-      <c r="AI34" s="11"/>
-      <c r="AJ34" s="11"/>
-      <c r="AK34" s="11"/>
+      <c r="AF34" s="10"/>
+      <c r="AG34" s="10"/>
+      <c r="AH34" s="10"/>
+      <c r="AI34" s="10"/>
+      <c r="AJ34" s="10"/>
+      <c r="AK34" s="10"/>
     </row>
     <row r="35" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y35" s="3"/>
@@ -6970,12 +6964,12 @@
       <c r="AB35" s="3"/>
       <c r="AD35" s="3"/>
       <c r="AE35" s="3"/>
-      <c r="AF35" s="11"/>
-      <c r="AG35" s="11"/>
-      <c r="AH35" s="11"/>
-      <c r="AI35" s="11"/>
-      <c r="AJ35" s="11"/>
-      <c r="AK35" s="11"/>
+      <c r="AF35" s="10"/>
+      <c r="AG35" s="10"/>
+      <c r="AH35" s="10"/>
+      <c r="AI35" s="10"/>
+      <c r="AJ35" s="10"/>
+      <c r="AK35" s="10"/>
     </row>
     <row r="36" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y36" s="3"/>
@@ -6984,12 +6978,12 @@
       <c r="AB36" s="3"/>
       <c r="AD36" s="3"/>
       <c r="AE36" s="3"/>
-      <c r="AF36" s="11"/>
-      <c r="AG36" s="11"/>
-      <c r="AH36" s="11"/>
-      <c r="AI36" s="11"/>
-      <c r="AJ36" s="11"/>
-      <c r="AK36" s="11"/>
+      <c r="AF36" s="10"/>
+      <c r="AG36" s="10"/>
+      <c r="AH36" s="10"/>
+      <c r="AI36" s="10"/>
+      <c r="AJ36" s="10"/>
+      <c r="AK36" s="10"/>
     </row>
     <row r="37" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y37" s="3"/>
@@ -6998,12 +6992,12 @@
       <c r="AB37" s="3"/>
       <c r="AD37" s="3"/>
       <c r="AE37" s="3"/>
-      <c r="AF37" s="11"/>
-      <c r="AG37" s="11"/>
-      <c r="AH37" s="11"/>
-      <c r="AI37" s="11"/>
-      <c r="AJ37" s="11"/>
-      <c r="AK37" s="11"/>
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="10"/>
+      <c r="AH37" s="10"/>
+      <c r="AI37" s="10"/>
+      <c r="AJ37" s="10"/>
+      <c r="AK37" s="10"/>
     </row>
     <row r="38" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y38" s="3"/>
@@ -7012,12 +7006,12 @@
       <c r="AB38" s="3"/>
       <c r="AD38" s="3"/>
       <c r="AE38" s="3"/>
-      <c r="AF38" s="11"/>
-      <c r="AG38" s="11"/>
-      <c r="AH38" s="11"/>
-      <c r="AI38" s="11"/>
-      <c r="AJ38" s="11"/>
-      <c r="AK38" s="11"/>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="10"/>
+      <c r="AH38" s="10"/>
+      <c r="AI38" s="10"/>
+      <c r="AJ38" s="10"/>
+      <c r="AK38" s="10"/>
     </row>
     <row r="39" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y39" s="3"/>
@@ -7026,12 +7020,12 @@
       <c r="AB39" s="3"/>
       <c r="AD39" s="3"/>
       <c r="AE39" s="3"/>
-      <c r="AF39" s="11"/>
-      <c r="AG39" s="11"/>
-      <c r="AH39" s="11"/>
-      <c r="AI39" s="11"/>
-      <c r="AJ39" s="11"/>
-      <c r="AK39" s="11"/>
+      <c r="AF39" s="10"/>
+      <c r="AG39" s="10"/>
+      <c r="AH39" s="10"/>
+      <c r="AI39" s="10"/>
+      <c r="AJ39" s="10"/>
+      <c r="AK39" s="10"/>
     </row>
     <row r="40" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y40" s="3"/>
@@ -7040,12 +7034,12 @@
       <c r="AB40" s="3"/>
       <c r="AD40" s="3"/>
       <c r="AE40" s="3"/>
-      <c r="AF40" s="11"/>
-      <c r="AG40" s="11"/>
-      <c r="AH40" s="11"/>
-      <c r="AI40" s="11"/>
-      <c r="AJ40" s="11"/>
-      <c r="AK40" s="11"/>
+      <c r="AF40" s="10"/>
+      <c r="AG40" s="10"/>
+      <c r="AH40" s="10"/>
+      <c r="AI40" s="10"/>
+      <c r="AJ40" s="10"/>
+      <c r="AK40" s="10"/>
     </row>
     <row r="41" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y41" s="3"/>
@@ -7054,12 +7048,12 @@
       <c r="AB41" s="3"/>
       <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
-      <c r="AF41" s="11"/>
-      <c r="AG41" s="11"/>
-      <c r="AH41" s="11"/>
-      <c r="AI41" s="11"/>
-      <c r="AJ41" s="11"/>
-      <c r="AK41" s="11"/>
+      <c r="AF41" s="10"/>
+      <c r="AG41" s="10"/>
+      <c r="AH41" s="10"/>
+      <c r="AI41" s="10"/>
+      <c r="AJ41" s="10"/>
+      <c r="AK41" s="10"/>
     </row>
     <row r="42" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y42" s="3"/>
@@ -7068,12 +7062,12 @@
       <c r="AB42" s="3"/>
       <c r="AD42" s="3"/>
       <c r="AE42" s="3"/>
-      <c r="AF42" s="11"/>
-      <c r="AG42" s="11"/>
-      <c r="AH42" s="11"/>
-      <c r="AI42" s="11"/>
-      <c r="AJ42" s="11"/>
-      <c r="AK42" s="11"/>
+      <c r="AF42" s="10"/>
+      <c r="AG42" s="10"/>
+      <c r="AH42" s="10"/>
+      <c r="AI42" s="10"/>
+      <c r="AJ42" s="10"/>
+      <c r="AK42" s="10"/>
     </row>
     <row r="43" spans="25:37" x14ac:dyDescent="0.25">
       <c r="Y43" s="3"/>
@@ -7112,23 +7106,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0084C9-45AB-4EE5-8155-D8D47B937B6A}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:G37"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.75" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.25" bestFit="1" customWidth="1"/>
@@ -7141,48 +7132,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>68</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>69</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>71</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>72</v>
       </c>
-      <c r="M1" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7">
@@ -7223,89 +7214,89 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="7">
+        <v>251.77777776666667</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.10419682057220052</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1.1464436653584047</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2.9325555218636379</v>
+      </c>
+      <c r="F3" s="7">
+        <v>6.3478540017203082</v>
+      </c>
+      <c r="G3" s="7">
+        <v>3.1193551097403404E-3</v>
+      </c>
+      <c r="H3" s="7">
+        <v>8.6831247203256745E-3</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1.444908855651305E-2</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1.151509140274018E-2</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0.11770471404381526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B4" s="7">
         <v>224.45415832500001</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C4" s="7">
         <v>0.10418928209581706</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D4" s="7">
         <v>1.2791062208410653</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E4" s="7">
         <v>2.9288176069844964</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F4" s="7">
         <v>15.229778570065298</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G4" s="7">
         <v>1.1929265056063339E-2</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H4" s="7">
         <v>5.2481238648807724E-3</v>
       </c>
-      <c r="I3" s="7">
-        <v>0</v>
-      </c>
-      <c r="J3" s="7">
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
         <v>2.4663493480429066E-2</v>
       </c>
-      <c r="K3" s="7">
-        <v>0</v>
-      </c>
-      <c r="L3" s="7">
-        <v>0</v>
-      </c>
-      <c r="M3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="7">
-        <v>251.77777776666667</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0.10419682057220052</v>
-      </c>
-      <c r="D4" s="7">
-        <v>1.1464436653584047</v>
-      </c>
-      <c r="E4" s="7">
-        <v>2.9325555218636379</v>
-      </c>
-      <c r="F4" s="7">
-        <v>6.3478540017203082</v>
-      </c>
-      <c r="G4" s="7">
-        <v>3.1193551097403404E-3</v>
-      </c>
-      <c r="H4" s="7">
-        <v>8.6831247203256745E-3</v>
-      </c>
-      <c r="I4" s="7">
-        <v>0</v>
-      </c>
-      <c r="J4" s="7">
-        <v>1.444908855651305E-2</v>
-      </c>
       <c r="K4" s="7">
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <v>1.151509140274018E-2</v>
+        <v>0</v>
       </c>
       <c r="M4" s="7">
-        <v>0.11770471404381526</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="7">
@@ -7346,7 +7337,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="7">
@@ -7387,34 +7378,34 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>63</v>
+      <c r="A8" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
         <v>80</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>81</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>82</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>83</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>84</v>
       </c>
-      <c r="G8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="7">
@@ -7435,27 +7426,27 @@
       <c r="G9" s="7">
         <v>50.801207231517402</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="K9" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="L9" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="M9" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="N9" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="N9" s="16" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="7">
@@ -7476,171 +7467,171 @@
       <c r="G10" s="7">
         <v>51.742383571055498</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" t="s">
         <v>92</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>93</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>94</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>95</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>96</v>
       </c>
-      <c r="N10" t="s">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="7">
+        <v>7.0379199722008314</v>
+      </c>
+      <c r="C11" s="7">
+        <v>12.7485380684519</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5.7885718190937192</v>
+      </c>
+      <c r="E11" s="7">
+        <v>5.3214697556331014</v>
+      </c>
+      <c r="F11" s="7">
+        <v>52.985617053546918</v>
+      </c>
+      <c r="G11" s="7">
+        <v>23.155803303274364</v>
+      </c>
+      <c r="I11" s="14" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="7">
+      <c r="J11" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="7">
+        <v>6.2233367292674222</v>
+      </c>
+      <c r="C12" s="7">
+        <v>13.966757988130531</v>
+      </c>
+      <c r="D12" s="7">
+        <v>6.3109753852480175</v>
+      </c>
+      <c r="E12" s="7">
+        <v>4.7169077450525529</v>
+      </c>
+      <c r="F12" s="7">
+        <v>49.971546943037644</v>
+      </c>
+      <c r="G12" s="7">
+        <v>25.033811938531251</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="16">
+        <v>256.42</v>
+      </c>
+      <c r="K12" s="16">
+        <v>254.4</v>
+      </c>
+      <c r="L12" s="16">
+        <v>284.48</v>
+      </c>
+      <c r="M12" s="16">
+        <v>282.45999999999998</v>
+      </c>
+      <c r="N12" s="16">
+        <v>280.44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="7">
         <v>1.7596708664456144</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C13" s="7">
         <v>20.011186422844034</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D13" s="7">
         <v>3.5405701957503477</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E13" s="7">
         <v>3.4713832623212095</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F13" s="7">
         <v>16.692622291928057</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G13" s="7">
         <v>56.284237827156346</v>
       </c>
-      <c r="I11" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="N11" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="7">
-        <v>7.0379199722008314</v>
-      </c>
-      <c r="C12" s="7">
-        <v>12.7485380684519</v>
-      </c>
-      <c r="D12" s="7">
-        <v>5.7885718190937192</v>
-      </c>
-      <c r="E12" s="7">
-        <v>5.3214697556331014</v>
-      </c>
-      <c r="F12" s="7">
-        <v>52.985617053546918</v>
-      </c>
-      <c r="G12" s="7">
-        <v>23.155803303274364</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="J12" s="17">
-        <v>256.42</v>
-      </c>
-      <c r="K12" s="17">
-        <v>254.4</v>
-      </c>
-      <c r="L12" s="17">
-        <v>284.48</v>
-      </c>
-      <c r="M12" s="17">
-        <v>282.45999999999998</v>
-      </c>
-      <c r="N12" s="17">
-        <v>280.44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="7">
-        <v>6.2233367292674222</v>
-      </c>
-      <c r="C13" s="7">
-        <v>13.966757988130531</v>
-      </c>
-      <c r="D13" s="7">
-        <v>6.3109753852480175</v>
-      </c>
-      <c r="E13" s="7">
-        <v>4.7169077450525529</v>
-      </c>
-      <c r="F13" s="7">
-        <v>49.971546943037644</v>
-      </c>
-      <c r="G13" s="7">
-        <v>25.033811938531251</v>
-      </c>
-      <c r="I13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="17"/>
+      <c r="I13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" s="14" t="s">
         <v>84</v>
-      </c>
-      <c r="F15" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="15">
         <f t="shared" ref="B16:F20" si="0">C9*J$12/SUMPRODUCT($C9:$G9,$J$12:$N$12)</f>
         <v>0.19708150113561135</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="15">
         <f t="shared" si="0"/>
         <v>6.3177938840151854E-2</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="15">
         <f t="shared" si="0"/>
         <v>3.6962306685441836E-2</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="15">
         <f t="shared" si="0"/>
         <v>0.1830339347399759</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="15">
         <f t="shared" si="0"/>
         <v>0.5197443185988192</v>
       </c>
@@ -7649,311 +7640,312 @@
       <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="15">
         <f t="shared" si="0"/>
         <v>0.15284287597246557</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="15">
         <f t="shared" si="0"/>
         <v>8.4984473978066744E-2</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="15">
         <f t="shared" si="0"/>
         <v>2.3203022303856981E-2</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="15">
         <f t="shared" si="0"/>
         <v>0.21058632029797503</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="15">
         <f t="shared" si="0"/>
         <v>0.52838330744763562</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18">
+        <v>173</v>
+      </c>
+      <c r="B18" s="15">
         <f t="shared" si="0"/>
-        <v>0.1864635745402132</v>
-      </c>
-      <c r="C18">
+        <v>0.11794740269865614</v>
+      </c>
+      <c r="C18" s="15">
         <f t="shared" si="0"/>
-        <v>3.273102365155562E-2</v>
-      </c>
-      <c r="D18">
+        <v>5.3133036210584177E-2</v>
+      </c>
+      <c r="D18" s="15">
         <f t="shared" si="0"/>
-        <v>3.5885877988085943E-2</v>
-      </c>
-      <c r="E18">
+        <v>5.4620973759245239E-2</v>
+      </c>
+      <c r="E18" s="15">
         <f t="shared" si="0"/>
-        <v>0.17133685589891903</v>
-      </c>
-      <c r="F18">
+        <v>0.53999663303088308</v>
+      </c>
+      <c r="F18" s="15">
         <f t="shared" si="0"/>
-        <v>0.57358266792122614</v>
+        <v>0.23430195430063122</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="15">
         <f t="shared" si="0"/>
-        <v>0.11794740269865614</v>
-      </c>
-      <c r="C19">
+        <v>0.1294582433761583</v>
+      </c>
+      <c r="C19" s="15">
         <f t="shared" si="0"/>
-        <v>5.3133036210584177E-2</v>
-      </c>
-      <c r="D19">
+        <v>5.8035776468512226E-2</v>
+      </c>
+      <c r="D19" s="15">
         <f t="shared" si="0"/>
-        <v>5.4620973759245239E-2</v>
-      </c>
-      <c r="E19">
+        <v>4.8505538182016882E-2</v>
+      </c>
+      <c r="E19" s="15">
         <f t="shared" si="0"/>
-        <v>0.53999663303088308</v>
-      </c>
-      <c r="F19">
+        <v>0.51022525885370418</v>
+      </c>
+      <c r="F19" s="15">
         <f t="shared" si="0"/>
-        <v>0.23430195430063122</v>
+        <v>0.25377518311960845</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="15">
+        <f>C13*J$12/SUMPRODUCT($C13:$G13,$J$12:$N$12)</f>
+        <v>0.1864635745402132</v>
+      </c>
+      <c r="C20" s="15">
         <f t="shared" si="0"/>
-        <v>0.1294582433761583</v>
-      </c>
-      <c r="C20">
+        <v>3.273102365155562E-2</v>
+      </c>
+      <c r="D20" s="15">
         <f t="shared" si="0"/>
-        <v>5.8035776468512226E-2</v>
-      </c>
-      <c r="D20">
+        <v>3.5885877988085943E-2</v>
+      </c>
+      <c r="E20" s="15">
         <f t="shared" si="0"/>
-        <v>4.8505538182016882E-2</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0.51022525885370418</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0.25377518311960845</v>
+        <v>0.17133685589891903</v>
+      </c>
+      <c r="F20" s="15">
+        <f>G13*N$12/SUMPRODUCT($C13:$G13,$J$12:$N$12)</f>
+        <v>0.57358266792122614</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" t="s">
         <v>93</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>94</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>95</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>96</v>
       </c>
-      <c r="F22" t="s">
-        <v>97</v>
-      </c>
       <c r="G22" t="s">
+        <v>158</v>
+      </c>
+      <c r="H22" t="s">
+        <v>107</v>
+      </c>
+      <c r="I22" t="s">
+        <v>139</v>
+      </c>
+      <c r="J22" t="s">
+        <v>108</v>
+      </c>
+      <c r="K22" t="s">
+        <v>148</v>
+      </c>
+      <c r="L22" t="s">
+        <v>150</v>
+      </c>
+      <c r="M22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" t="s">
         <v>159</v>
       </c>
-      <c r="H22" t="s">
-        <v>108</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="H23" t="s">
+        <v>136</v>
+      </c>
+      <c r="I23" t="s">
         <v>140</v>
       </c>
-      <c r="J22" t="s">
-        <v>109</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="J23" t="s">
+        <v>143</v>
+      </c>
+      <c r="K23" t="s">
+        <v>146</v>
+      </c>
+      <c r="L23" t="s">
+        <v>151</v>
+      </c>
+      <c r="M23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" t="s">
+        <v>160</v>
+      </c>
+      <c r="H24" t="s">
+        <v>137</v>
+      </c>
+      <c r="I24" t="s">
+        <v>141</v>
+      </c>
+      <c r="J24" t="s">
+        <v>144</v>
+      </c>
+      <c r="K24" t="s">
+        <v>147</v>
+      </c>
+      <c r="L24" t="s">
+        <v>152</v>
+      </c>
+      <c r="M24" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" t="s">
+        <v>133</v>
+      </c>
+      <c r="G25" t="s">
+        <v>161</v>
+      </c>
+      <c r="H25" t="s">
+        <v>138</v>
+      </c>
+      <c r="I25" t="s">
+        <v>142</v>
+      </c>
+      <c r="J25" t="s">
+        <v>145</v>
+      </c>
+      <c r="K25" t="s">
         <v>149</v>
       </c>
-      <c r="L22" t="s">
-        <v>151</v>
-      </c>
-      <c r="M22" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" t="s">
-        <v>112</v>
-      </c>
-      <c r="C23" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" t="s">
-        <v>122</v>
-      </c>
-      <c r="E23" t="s">
-        <v>127</v>
-      </c>
-      <c r="F23" t="s">
-        <v>132</v>
-      </c>
-      <c r="G23" t="s">
-        <v>160</v>
-      </c>
-      <c r="H23" t="s">
-        <v>137</v>
-      </c>
-      <c r="I23" t="s">
-        <v>141</v>
-      </c>
-      <c r="J23" t="s">
-        <v>144</v>
-      </c>
-      <c r="K23" t="s">
-        <v>147</v>
-      </c>
-      <c r="L23" t="s">
-        <v>152</v>
-      </c>
-      <c r="M23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24" t="s">
-        <v>123</v>
-      </c>
-      <c r="E24" t="s">
-        <v>128</v>
-      </c>
-      <c r="F24" t="s">
-        <v>133</v>
-      </c>
-      <c r="G24" t="s">
-        <v>161</v>
-      </c>
-      <c r="H24" t="s">
-        <v>138</v>
-      </c>
-      <c r="I24" t="s">
-        <v>142</v>
-      </c>
-      <c r="J24" t="s">
-        <v>145</v>
-      </c>
-      <c r="K24" t="s">
-        <v>148</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="L25" t="s">
         <v>153</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M25" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>115</v>
-      </c>
-      <c r="C25" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" t="s">
-        <v>124</v>
-      </c>
-      <c r="E25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F25" t="s">
-        <v>134</v>
-      </c>
-      <c r="G25" t="s">
-        <v>162</v>
-      </c>
-      <c r="H25" t="s">
-        <v>139</v>
-      </c>
-      <c r="I25" t="s">
-        <v>143</v>
-      </c>
-      <c r="J25" t="s">
-        <v>146</v>
-      </c>
-      <c r="K25" t="s">
-        <v>150</v>
-      </c>
-      <c r="L25" t="s">
-        <v>154</v>
-      </c>
-      <c r="M25" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -7983,43 +7975,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
       <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
-        <v>66</v>
-      </c>
       <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>78</v>
       </c>
-      <c r="L1" t="s">
-        <v>79</v>
-      </c>
       <c r="M1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -8079,35 +8071,35 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'Pivot tables'!A3</f>
-        <v>JFYL18</v>
+        <v>JFYL14</v>
       </c>
       <c r="B3" s="7">
         <f>'Pivot tables'!B3/1000</f>
-        <v>0.22445415832500001</v>
+        <v>0.25177777776666665</v>
       </c>
       <c r="C3" s="7">
         <f>'Pivot tables'!C3</f>
-        <v>0.10418928209581706</v>
+        <v>0.10419682057220052</v>
       </c>
       <c r="D3" s="7">
         <f>-'Pivot tables'!D3</f>
-        <v>-1.2791062208410653</v>
+        <v>-1.1464436653584047</v>
       </c>
       <c r="E3" s="7">
         <f>'Pivot tables'!E3</f>
-        <v>2.9288176069844964</v>
+        <v>2.9325555218636379</v>
       </c>
       <c r="F3" s="7">
         <f>-'Pivot tables'!F3</f>
-        <v>-15.229778570065298</v>
+        <v>-6.3478540017203082</v>
       </c>
       <c r="G3" s="7">
         <f>'Pivot tables'!G3</f>
-        <v>1.1929265056063339E-2</v>
+        <v>3.1193551097403404E-3</v>
       </c>
       <c r="H3" s="7">
         <f>'Pivot tables'!H3</f>
-        <v>5.2481238648807724E-3</v>
+        <v>8.6831247203256745E-3</v>
       </c>
       <c r="I3" s="7">
         <f>'Pivot tables'!I3</f>
@@ -8115,7 +8107,7 @@
       </c>
       <c r="J3" s="7">
         <f>'Pivot tables'!J3</f>
-        <v>2.4663493480429066E-2</v>
+        <v>1.444908855651305E-2</v>
       </c>
       <c r="K3" s="7">
         <f>'Pivot tables'!K3</f>
@@ -8123,45 +8115,45 @@
       </c>
       <c r="L3" s="7">
         <f>'Pivot tables'!L3</f>
-        <v>0</v>
+        <v>1.151509140274018E-2</v>
       </c>
       <c r="M3" s="7">
         <f>'Pivot tables'!M3</f>
-        <v>0</v>
+        <v>0.11770471404381526</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'Pivot tables'!A4</f>
-        <v>JFYL66</v>
+        <v>JFYL18</v>
       </c>
       <c r="B4" s="7">
         <f>'Pivot tables'!B4/1000</f>
-        <v>0.25177777776666665</v>
+        <v>0.22445415832500001</v>
       </c>
       <c r="C4" s="7">
         <f>'Pivot tables'!C4</f>
-        <v>0.10419682057220052</v>
+        <v>0.10418928209581706</v>
       </c>
       <c r="D4" s="7">
         <f>-'Pivot tables'!D4</f>
-        <v>-1.1464436653584047</v>
+        <v>-1.2791062208410653</v>
       </c>
       <c r="E4" s="7">
         <f>'Pivot tables'!E4</f>
-        <v>2.9325555218636379</v>
+        <v>2.9288176069844964</v>
       </c>
       <c r="F4" s="7">
         <f>-'Pivot tables'!F4</f>
-        <v>-6.3478540017203082</v>
+        <v>-15.229778570065298</v>
       </c>
       <c r="G4" s="7">
         <f>'Pivot tables'!G4</f>
-        <v>3.1193551097403404E-3</v>
+        <v>1.1929265056063339E-2</v>
       </c>
       <c r="H4" s="7">
         <f>'Pivot tables'!H4</f>
-        <v>8.6831247203256745E-3</v>
+        <v>5.2481238648807724E-3</v>
       </c>
       <c r="I4" s="7">
         <f>'Pivot tables'!I4</f>
@@ -8169,7 +8161,7 @@
       </c>
       <c r="J4" s="7">
         <f>'Pivot tables'!J4</f>
-        <v>1.444908855651305E-2</v>
+        <v>2.4663493480429066E-2</v>
       </c>
       <c r="K4" s="7">
         <f>'Pivot tables'!K4</f>
@@ -8177,11 +8169,11 @@
       </c>
       <c r="L4" s="7">
         <f>'Pivot tables'!L4</f>
-        <v>1.151509140274018E-2</v>
+        <v>0</v>
       </c>
       <c r="M4" s="7">
         <f>'Pivot tables'!M4</f>
-        <v>0.11770471404381526</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -8301,8 +8293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DE8210-B7CB-4AB7-9EA7-8B7E7EFAFB50}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8314,26 +8306,26 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="str">
         <f>'Pivot tables'!B8</f>
         <v>lipidCont</v>
       </c>
       <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>89</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>90</v>
-      </c>
-      <c r="G1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -8399,91 +8391,91 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'Pivot tables'!A11</f>
-        <v>JFYL66</v>
+        <v>OKYL029</v>
       </c>
       <c r="B4" s="7">
         <f>'Pivot tables'!B11/100</f>
-        <v>1.7596708664456145E-2</v>
+        <v>7.0379199722008318E-2</v>
       </c>
       <c r="C4" s="7">
         <f>'Pivot tables'!B18</f>
-        <v>0.1864635745402132</v>
+        <v>0.11794740269865614</v>
       </c>
       <c r="D4" s="7">
         <f>'Pivot tables'!C18</f>
-        <v>3.273102365155562E-2</v>
+        <v>5.3133036210584177E-2</v>
       </c>
       <c r="E4" s="7">
         <f>'Pivot tables'!D18</f>
-        <v>3.5885877988085943E-2</v>
+        <v>5.4620973759245239E-2</v>
       </c>
       <c r="F4" s="7">
         <f>'Pivot tables'!E18</f>
-        <v>0.17133685589891903</v>
+        <v>0.53999663303088308</v>
       </c>
       <c r="G4" s="7">
         <f>'Pivot tables'!F18</f>
-        <v>0.57358266792122614</v>
+        <v>0.23430195430063122</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'Pivot tables'!A12</f>
-        <v>OKYL029</v>
+        <v>ST6512</v>
       </c>
       <c r="B5" s="7">
         <f>'Pivot tables'!B12/100</f>
-        <v>7.0379199722008318E-2</v>
+        <v>6.2233367292674223E-2</v>
       </c>
       <c r="C5" s="7">
         <f>'Pivot tables'!B19</f>
-        <v>0.11794740269865614</v>
+        <v>0.1294582433761583</v>
       </c>
       <c r="D5" s="7">
         <f>'Pivot tables'!C19</f>
-        <v>5.3133036210584177E-2</v>
+        <v>5.8035776468512226E-2</v>
       </c>
       <c r="E5" s="7">
         <f>'Pivot tables'!D19</f>
-        <v>5.4620973759245239E-2</v>
+        <v>4.8505538182016882E-2</v>
       </c>
       <c r="F5" s="7">
         <f>'Pivot tables'!E19</f>
-        <v>0.53999663303088308</v>
+        <v>0.51022525885370418</v>
       </c>
       <c r="G5" s="7">
         <f>'Pivot tables'!F19</f>
-        <v>0.23430195430063122</v>
+        <v>0.25377518311960845</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>'Pivot tables'!A13</f>
-        <v>ST6512</v>
+        <v>JFYL14</v>
       </c>
       <c r="B6" s="7">
         <f>'Pivot tables'!B13/100</f>
-        <v>6.2233367292674223E-2</v>
+        <v>1.7596708664456145E-2</v>
       </c>
       <c r="C6" s="7">
         <f>'Pivot tables'!B20</f>
-        <v>0.1294582433761583</v>
+        <v>0.1864635745402132</v>
       </c>
       <c r="D6" s="7">
         <f>'Pivot tables'!C20</f>
-        <v>5.8035776468512226E-2</v>
+        <v>3.273102365155562E-2</v>
       </c>
       <c r="E6" s="7">
         <f>'Pivot tables'!D20</f>
-        <v>4.8505538182016882E-2</v>
+        <v>3.5885877988085943E-2</v>
       </c>
       <c r="F6" s="7">
         <f>'Pivot tables'!E20</f>
-        <v>0.51022525885370418</v>
+        <v>0.17133685589891903</v>
       </c>
       <c r="G6" s="7">
         <f>'Pivot tables'!F20</f>
-        <v>0.25377518311960845</v>
+        <v>0.57358266792122614</v>
       </c>
     </row>
   </sheetData>
@@ -8495,7 +8487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{652CE5F1-2D30-4A5F-8B3E-F698942F7C27}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
@@ -8512,209 +8504,209 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" t="s">
         <v>108</v>
       </c>
-      <c r="C1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" t="s">
-        <v>109</v>
-      </c>
       <c r="E1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>